<commit_message>
Update notebooks ands reports
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada-Coimbra-cargos_tarefas.xlsx
+++ b/notebooks/jesuita-entrada-Coimbra-cargos_tarefas.xlsx
@@ -926,12 +926,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Funda a residência jesuíta de Macau</t>
+          <t>Superior de Macau</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -958,12 +958,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Superior de Macau</t>
+          <t>Funda a residência jesuíta de Macau</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1876,22 +1876,22 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-rodrigues-girao</t>
+          <t>deh-nicolau-pimenta</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>João Rodrigues Girão</t>
+          <t>Nicolau Pimenta</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Carta anual do Japão</t>
+          <t>Visitador das Índias Orientais</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1908,22 +1908,22 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>deh-nicolau-pimenta</t>
+          <t>deh-joao-rodrigues-girao</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Nicolau Pimenta</t>
+          <t>João Rodrigues Girão</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Visitador das Índias Orientais</t>
+          <t>Carta anual do Japão</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2324,17 +2324,17 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pacheco</t>
+          <t>deh-mateus-de-couros</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Francisco Pacheco</t>
+          <t>Mateus de Couros</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Provincial do Japão e da China</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2356,17 +2356,17 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>deh-mateus-de-couros</t>
+          <t>deh-francisco-pacheco</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Mateus de Couros</t>
+          <t>Francisco Pacheco</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Provincial do Japão e da China</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2420,17 +2420,17 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pacheco</t>
+          <t>deh-manuel-dias-o-novo</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Francisco Pacheco</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Superior da missão da China</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2452,22 +2452,22 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>deh-gaspar-do-amaral</t>
+          <t>deh-francisco-pacheco</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Francisco Pacheco</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Faz mais de 40000 baptismos no Tonquim</t>
+          <t>Superior da missão da China</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2484,22 +2484,22 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-dias-o-novo</t>
+          <t>deh-gaspar-do-amaral</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Faz mais de 40000 baptismos no Tonquim</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2676,17 +2676,17 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>deh-andre-palmeiro</t>
+          <t>deh-mateus-de-couros</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>André Palmeiro</t>
+          <t>Mateus de Couros</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Visitador das províncias de Goa e do Malabar</t>
+          <t>Provincial do Japão e da China</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Visitador das províncias de Goa e do Malabar</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2740,22 +2740,22 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-rodrigues-girao</t>
+          <t>deh-andre-palmeiro</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>João Rodrigues Girão</t>
+          <t>André Palmeiro</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Carta anual do Japão</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2772,22 +2772,22 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>deh-mateus-de-couros</t>
+          <t>deh-joao-rodrigues-girao</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Mateus de Couros</t>
+          <t>João Rodrigues Girão</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Provincial do Japão e da China</t>
+          <t>Carta anual do Japão</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2836,17 +2836,17 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-andrade</t>
+          <t>deh-gaspar-do-amaral</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Provincial de Goa</t>
+          <t>Superior da missão do Tonquim</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2868,17 +2868,17 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>deh-gaspar-do-amaral</t>
+          <t>deh-antonio-de-andrade</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Superior da missão do Tonquim</t>
+          <t>Provincial de Goa</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2996,17 +2996,17 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>deh-andre-palmeiro</t>
+          <t>deh-manuel-dias-o-novo</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>André Palmeiro</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3060,17 +3060,17 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-dias-o-novo</t>
+          <t>deh-andre-palmeiro</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>André Palmeiro</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3444,17 +3444,17 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-furtado</t>
+          <t>deh-manuel-dias-o-novo</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Superior das seis residências do Norte</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3476,17 +3476,17 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-dias-o-novo</t>
+          <t>deh-francisco-furtado</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Superior das seis residências do Norte</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3764,17 +3764,17 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>deh-matias-da-maia</t>
+          <t>deh-simao-da-cunha</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3796,17 +3796,17 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>deh-sebastiao-da-maia</t>
+          <t>deh-matias-da-maia</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3828,17 +3828,17 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>deh-simao-da-cunha</t>
+          <t>deh-sebastiao-da-maia</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4340,22 +4340,22 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-de-sa</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Manuel de Sá</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Enviado ao rei</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -4372,22 +4372,22 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-manuel-de-sa</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Manuel de Sá</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Enviado ao rei</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -4500,17 +4500,17 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-da-silva</t>
+          <t>deh-leonardo-teixeira</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>António da Silva</t>
+          <t>Leonardo Teixeira</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Reitor de Nanquim</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4532,17 +4532,17 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>deh-leonardo-teixeira</t>
+          <t>deh-antonio-da-silva</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Leonardo Teixeira</t>
+          <t>António da Silva</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Reitor de Nanquim</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4628,22 +4628,22 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>deh-leonardo-teixeira</t>
+          <t>deh-manuel-osorio-i</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Leonardo Teixeira</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Sai da Companhia</t>
+          <t>Reitor do colégio de Macau</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>jesuita-tarefa</t>
+          <t>jesuita-cargo</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -4670,7 +4670,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Reitor do colégio de Macau</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4692,17 +4692,17 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-osorio-i</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4724,22 +4724,22 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-leonardo-teixeira</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Leonardo Teixeira</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Sai da Companhia</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>jesuita-cargo</t>
+          <t>jesuita-tarefa</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -4788,17 +4788,17 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pinto-i</t>
+          <t>deh-manuel-osorio-i</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4830,7 +4830,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Procurador da Província do Japão em Macau</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4852,17 +4852,17 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-osorio-i</t>
+          <t>deh-francisco-pinto-i</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Procurador da Província do Japão em Macau</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4980,12 +4980,12 @@
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pinto-i</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5012,12 +5012,12 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-francisco-pinto-i</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5076,12 +5076,12 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-da-silva</t>
+          <t>deh-manuel-mendes</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>António da Silva</t>
+          <t>Manuel Mendes</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5108,12 +5108,12 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-mendes</t>
+          <t>deh-antonio-da-silva</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Manuel Mendes</t>
+          <t>António da Silva</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5236,17 +5236,17 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>deh-estanislau-machado</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Estanislau Machado</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Superior da missão do Tonquim</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Superior da missão do Tonquim</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -5300,12 +5300,12 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-estanislau-machado</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Estanislau Machado</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5460,17 +5460,17 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pinto-i</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -5492,17 +5492,17 @@
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pinto-i</t>
+          <t>deh-manuel-mendes</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Manuel Mendes</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Vice-visitador do Japão</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -5524,17 +5524,17 @@
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-mendes</t>
+          <t>deh-francisco-pinto-i</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Manuel Mendes</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -5556,17 +5556,17 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-francisco-pinto-i</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Vice-visitador do Japão</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">

</xml_diff>